<commit_message>
naam naar medex veranderd en kleine aanpassingen
</commit_message>
<xml_diff>
--- a/Documentatie/Fase 3/Genormaliseerd_databaseontwerp.xlsx
+++ b/Documentatie/Fase 3/Genormaliseerd_databaseontwerp.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
   <si>
     <t>0ste normaalvorm</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>UserId</t>
-  </si>
-  <si>
-    <t>taskId</t>
   </si>
   <si>
     <t>UserMeta</t>
@@ -1112,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51:F53"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,7 +1196,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1259,17 +1256,17 @@
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -1280,7 +1277,7 @@
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E31" t="s">
@@ -1291,8 +1288,8 @@
       <c r="A32" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>25</v>
+      <c r="C32" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
@@ -1348,20 +1345,20 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E52" s="9"/>
       <c r="F52" s="10"/>
@@ -1372,7 +1369,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -1407,13 +1404,13 @@
       <c r="B68" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>27</v>
+      <c r="D68" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C71" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>